<commit_message>
iOS Android DataFrame Merge Issue Fix
</commit_message>
<xml_diff>
--- a/combinedRatings.xlsx
+++ b/combinedRatings.xlsx
@@ -488,27 +488,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>My altafiber</t>
+          <t>Go Kinetic by Windstream</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.5</v>
+        <v>4.65</v>
       </c>
       <c r="D2" t="n">
-        <v>4710</v>
+        <v>82788</v>
       </c>
       <c r="E2" t="n">
         <v>4.8</v>
       </c>
       <c r="F2" t="n">
-        <v>4393</v>
+        <v>61742</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="I2" t="n">
-        <v>317</v>
+        <v>21046</v>
       </c>
     </row>
     <row r="3">
@@ -519,27 +519,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>My Sprint Mobile</t>
+          <t>My altafiber</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1237634</v>
+        <v>4743</v>
       </c>
       <c r="E3" t="n">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="F3" t="n">
-        <v>1047309</v>
+        <v>4426</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>4.1</v>
+        <v>4.2</v>
       </c>
       <c r="I3" t="n">
-        <v>190325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4">
@@ -550,27 +550,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MyDISH Account</t>
+          <t>Spectrum Access: Enabled Media</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4.1</v>
+        <v>4.5</v>
       </c>
       <c r="D4" t="n">
-        <v>1096771</v>
+        <v>265</v>
       </c>
       <c r="E4" t="n">
-        <v>4.6</v>
+        <v>4.5</v>
       </c>
       <c r="F4" t="n">
-        <v>322194</v>
+        <v>123</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="I4" t="n">
-        <v>774577</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5">
@@ -581,29 +581,29 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>My CenturyLink</t>
+          <t>Cox App</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>4.55</v>
       </c>
       <c r="D5" t="n">
-        <v>175671</v>
+        <v>489344</v>
       </c>
       <c r="E5" t="n">
-        <v>4.4</v>
+        <v>4.6</v>
       </c>
       <c r="F5" t="n">
-        <v>116043</v>
+        <v>399031</v>
       </c>
       <c r="G5" t="n">
-        <v>196</v>
+        <v>117</v>
       </c>
       <c r="H5" t="n">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="I5" t="n">
-        <v>59628</v>
+        <v>90313</v>
       </c>
     </row>
     <row r="6">
@@ -614,29 +614,29 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>T-Mobile</t>
+          <t>My Verizon</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4.449999999999999</v>
+        <v>4.6</v>
       </c>
       <c r="D6" t="n">
-        <v>2556296</v>
+        <v>5750786</v>
       </c>
       <c r="E6" t="n">
-        <v>4.8</v>
+        <v>4.6</v>
       </c>
       <c r="F6" t="n">
-        <v>2412812</v>
+        <v>4754388</v>
       </c>
       <c r="G6" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H6" t="n">
-        <v>4.1</v>
+        <v>4.6</v>
       </c>
       <c r="I6" t="n">
-        <v>143484</v>
+        <v>996398</v>
       </c>
     </row>
     <row r="7">
@@ -647,29 +647,29 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>My Spectrum</t>
+          <t>myCricket App</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>4.55</v>
+        <v>4.3</v>
       </c>
       <c r="D7" t="n">
-        <v>2086809</v>
+        <v>233477</v>
       </c>
       <c r="E7" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="F7" t="n">
-        <v>2010064</v>
+        <v>43149</v>
       </c>
       <c r="G7" t="n">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="H7" t="n">
-        <v>4.3</v>
+        <v>4.1</v>
       </c>
       <c r="I7" t="n">
-        <v>76745</v>
+        <v>190328</v>
       </c>
     </row>
     <row r="8">
@@ -680,29 +680,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Spectrum News: Local Stories</t>
+          <t>MyDISH Account</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.65</v>
+        <v>4.1</v>
       </c>
       <c r="D8" t="n">
-        <v>1021351</v>
+        <v>381866</v>
       </c>
       <c r="E8" t="n">
-        <v>4.7</v>
+        <v>4.6</v>
       </c>
       <c r="F8" t="n">
-        <v>24958</v>
-      </c>
-      <c r="G8" t="n">
-        <v>51</v>
-      </c>
+        <v>322237</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>4.6</v>
+        <v>3.6</v>
       </c>
       <c r="I8" t="n">
-        <v>996393</v>
+        <v>59629</v>
       </c>
     </row>
     <row r="9">
@@ -713,29 +711,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cox App</t>
+          <t>T-Mobile</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4.55</v>
+        <v>4.2</v>
       </c>
       <c r="D9" t="n">
-        <v>399173</v>
+        <v>3187389</v>
       </c>
       <c r="E9" t="n">
-        <v>4.6</v>
+        <v>4.8</v>
       </c>
       <c r="F9" t="n">
-        <v>399031</v>
+        <v>2412812</v>
       </c>
       <c r="G9" t="n">
-        <v>117</v>
+        <v>4</v>
       </c>
       <c r="H9" t="n">
-        <v>4.5</v>
+        <v>3.6</v>
       </c>
       <c r="I9" t="n">
-        <v>142</v>
+        <v>774577</v>
       </c>
     </row>
     <row r="10">
@@ -746,27 +744,29 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Spectrum Access: Enabled Media</t>
+          <t>Xfinity Mobile</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>55476</v>
+        <v>55397</v>
       </c>
       <c r="E10" t="n">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="F10" t="n">
-        <v>123</v>
-      </c>
-      <c r="G10" t="inlineStr"/>
+        <v>42796</v>
+      </c>
+      <c r="G10" t="n">
+        <v>87</v>
+      </c>
       <c r="H10" t="n">
-        <v>4.1</v>
+        <v>3.2</v>
       </c>
       <c r="I10" t="n">
-        <v>55353</v>
+        <v>12601</v>
       </c>
     </row>
     <row r="11">
@@ -777,29 +777,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Verizon My Fios</t>
+          <t>Spectrum News: Local Stories</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.85</v>
+        <v>4.4</v>
       </c>
       <c r="D11" t="n">
-        <v>270661</v>
+        <v>30351</v>
       </c>
       <c r="E11" t="n">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="F11" t="n">
-        <v>258060</v>
+        <v>24958</v>
       </c>
       <c r="G11" t="n">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="H11" t="n">
-        <v>3.2</v>
+        <v>4.1</v>
       </c>
       <c r="I11" t="n">
-        <v>12601</v>
+        <v>5393</v>
       </c>
     </row>
     <row r="12">
@@ -810,29 +810,29 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Xfinity Mobile</t>
+          <t>My Spectrum</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4.449999999999999</v>
+        <v>4.699999999999999</v>
       </c>
       <c r="D12" t="n">
-        <v>48189</v>
+        <v>2645951</v>
       </c>
       <c r="E12" t="n">
         <v>4.8</v>
       </c>
       <c r="F12" t="n">
-        <v>42796</v>
+        <v>2010064</v>
       </c>
       <c r="G12" t="n">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="H12" t="n">
-        <v>4.1</v>
+        <v>4.6</v>
       </c>
       <c r="I12" t="n">
-        <v>5393</v>
+        <v>635887</v>
       </c>
     </row>
     <row r="13">
@@ -843,27 +843,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Go Kinetic by Windstream</t>
+          <t>My Sprint Mobile</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4.65</v>
+        <v>4.3</v>
       </c>
       <c r="D13" t="n">
-        <v>152049</v>
+        <v>1190791</v>
       </c>
       <c r="E13" t="n">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="F13" t="n">
-        <v>61742</v>
+        <v>1047309</v>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
-        <v>4.5</v>
+        <v>4.1</v>
       </c>
       <c r="I13" t="n">
-        <v>90307</v>
+        <v>143482</v>
       </c>
     </row>
     <row r="14">
@@ -874,29 +874,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>myAT&amp;amp;T</t>
+          <t>Verizon My Fios</t>
         </is>
       </c>
       <c r="C14" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D14" t="n">
+        <v>334805</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F14" t="n">
+        <v>258060</v>
+      </c>
+      <c r="G14" t="n">
+        <v>111</v>
+      </c>
+      <c r="H14" t="n">
         <v>4.3</v>
       </c>
-      <c r="D14" t="n">
-        <v>4627173</v>
-      </c>
-      <c r="E14" t="n">
-        <v>4</v>
-      </c>
-      <c r="F14" t="n">
-        <v>3991303</v>
-      </c>
-      <c r="G14" t="n">
-        <v>14</v>
-      </c>
-      <c r="H14" t="n">
-        <v>4.6</v>
-      </c>
       <c r="I14" t="n">
-        <v>635870</v>
+        <v>76745</v>
       </c>
     </row>
     <row r="15">
@@ -907,29 +907,29 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>My Verizon</t>
+          <t>My CenturyLink</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4.55</v>
+        <v>4.25</v>
       </c>
       <c r="D15" t="n">
-        <v>4775434</v>
+        <v>171396</v>
       </c>
       <c r="E15" t="n">
-        <v>4.6</v>
+        <v>4.4</v>
       </c>
       <c r="F15" t="n">
-        <v>4754388</v>
+        <v>116043</v>
       </c>
       <c r="G15" t="n">
-        <v>9</v>
+        <v>196</v>
       </c>
       <c r="H15" t="n">
-        <v>4.5</v>
+        <v>4.1</v>
       </c>
       <c r="I15" t="n">
-        <v>21046</v>
+        <v>55353</v>
       </c>
     </row>
     <row r="16">
@@ -940,29 +940,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Spectrum TV</t>
+          <t>Visible mobile</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>4.45</v>
+        <v>4.300000000000001</v>
       </c>
       <c r="D16" t="n">
-        <v>441242</v>
+        <v>106650</v>
       </c>
       <c r="E16" t="n">
-        <v>4.7</v>
+        <v>4.4</v>
       </c>
       <c r="F16" t="n">
-        <v>411629</v>
+        <v>77035</v>
       </c>
       <c r="G16" t="n">
-        <v>47</v>
+        <v>156</v>
       </c>
       <c r="H16" t="n">
         <v>4.2</v>
       </c>
       <c r="I16" t="n">
-        <v>29613</v>
+        <v>29615</v>
       </c>
     </row>
     <row r="17">
@@ -973,20 +973,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>MediacomConnect</t>
+          <t>SpectrumU</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3.9</v>
+        <v>4.4</v>
       </c>
       <c r="D17" t="n">
-        <v>6855</v>
+        <v>427</v>
       </c>
       <c r="E17" t="n">
-        <v>3.3</v>
+        <v>4.3</v>
       </c>
       <c r="F17" t="n">
-        <v>6603</v>
+        <v>175</v>
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
@@ -1004,29 +1004,29 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Visible mobile</t>
+          <t>Spectrum TV</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3.85</v>
+        <v>4.65</v>
       </c>
       <c r="D18" t="n">
-        <v>78451</v>
+        <v>600878</v>
       </c>
       <c r="E18" t="n">
-        <v>4.4</v>
+        <v>4.7</v>
       </c>
       <c r="F18" t="n">
-        <v>77035</v>
+        <v>411629</v>
       </c>
       <c r="G18" t="n">
-        <v>156</v>
+        <v>47</v>
       </c>
       <c r="H18" t="n">
-        <v>3.3</v>
+        <v>4.6</v>
       </c>
       <c r="I18" t="n">
-        <v>1416</v>
+        <v>189249</v>
       </c>
     </row>
     <row r="19">
@@ -1037,23 +1037,29 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SpectrumU</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
+          <t>myAT&amp;amp;T</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>3.5</v>
+      </c>
       <c r="D19" t="n">
-        <v>175</v>
+        <v>4268811</v>
       </c>
       <c r="E19" t="n">
-        <v>4.3</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
-        <v>175</v>
-      </c>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+        <v>3991303</v>
+      </c>
+      <c r="G19" t="n">
+        <v>14</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3</v>
+      </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>277508</v>
       </c>
     </row>
     <row r="20">
@@ -1064,29 +1070,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Xfinity</t>
+          <t>Spectrum SportsNet: Live Games</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4.25</v>
+        <v>3.95</v>
       </c>
       <c r="D20" t="n">
-        <v>877434</v>
+        <v>5565</v>
       </c>
       <c r="E20" t="n">
-        <v>4.4</v>
+        <v>4.6</v>
       </c>
       <c r="F20" t="n">
-        <v>876975</v>
-      </c>
-      <c r="G20" t="n">
-        <v>5</v>
-      </c>
+        <v>4149</v>
+      </c>
+      <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
-        <v>4.1</v>
+        <v>3.3</v>
       </c>
       <c r="I20" t="n">
-        <v>459</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="21">
@@ -1097,27 +1101,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>HughesNet Mobile</t>
+          <t>MediacomConnect</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2.85</v>
+        <v>3.4</v>
       </c>
       <c r="D21" t="n">
-        <v>1460</v>
+        <v>19121</v>
       </c>
       <c r="E21" t="n">
-        <v>1.8</v>
+        <v>3.3</v>
       </c>
       <c r="F21" t="n">
-        <v>307</v>
+        <v>6603</v>
       </c>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
       <c r="I21" t="n">
-        <v>1153</v>
+        <v>12518</v>
       </c>
     </row>
     <row r="22">
@@ -1135,7 +1139,7 @@
         <v>3.4</v>
       </c>
       <c r="D22" t="n">
-        <v>382793</v>
+        <v>382796</v>
       </c>
       <c r="E22" t="n">
         <v>2.8</v>
@@ -1150,7 +1154,7 @@
         <v>4</v>
       </c>
       <c r="I22" t="n">
-        <v>379632</v>
+        <v>379635</v>
       </c>
     </row>
     <row r="23">
@@ -1168,7 +1172,7 @@
         <v>4.300000000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>81558</v>
+        <v>81559</v>
       </c>
       <c r="E23" t="n">
         <v>4.4</v>
@@ -1183,7 +1187,7 @@
         <v>4.2</v>
       </c>
       <c r="I23" t="n">
-        <v>36337</v>
+        <v>36338</v>
       </c>
     </row>
     <row r="24">
@@ -1194,27 +1198,29 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>My Viasat</t>
+          <t>Xfinity</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D24" t="n">
-        <v>3158</v>
+        <v>1030498</v>
       </c>
       <c r="E24" t="n">
-        <v>4.2</v>
+        <v>4.4</v>
       </c>
       <c r="F24" t="n">
-        <v>1620</v>
-      </c>
-      <c r="G24" t="inlineStr"/>
+        <v>876975</v>
+      </c>
+      <c r="G24" t="n">
+        <v>5</v>
+      </c>
       <c r="H24" t="n">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="I24" t="n">
-        <v>1538</v>
+        <v>153523</v>
       </c>
     </row>
     <row r="25">
@@ -1225,27 +1231,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Armstrong</t>
+          <t>Google Fiber</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3.35</v>
+        <v>3.75</v>
       </c>
       <c r="D25" t="n">
-        <v>277525</v>
+        <v>1444</v>
       </c>
       <c r="E25" t="n">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="F25" t="n">
-        <v>14</v>
+        <v>291</v>
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
-        <v>3</v>
+        <v>3.9</v>
       </c>
       <c r="I25" t="n">
-        <v>277511</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="26">
@@ -1256,27 +1262,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Optimum Support</t>
+          <t>My Viasat</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2.45</v>
+        <v>3.9</v>
       </c>
       <c r="D26" t="n">
-        <v>13893</v>
+        <v>4574</v>
       </c>
       <c r="E26" t="n">
-        <v>1.4</v>
+        <v>4.2</v>
       </c>
       <c r="F26" t="n">
-        <v>1375</v>
+        <v>1620</v>
       </c>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="I26" t="n">
-        <v>12518</v>
+        <v>2954</v>
       </c>
     </row>
     <row r="27">
@@ -1287,27 +1293,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Midco My Account</t>
+          <t>Armstrong</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2.95</v>
+        <v>3.9</v>
       </c>
       <c r="D27" t="n">
-        <v>189268</v>
+        <v>473</v>
       </c>
       <c r="E27" t="n">
-        <v>1.3</v>
+        <v>3.7</v>
       </c>
       <c r="F27" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="n">
-        <v>4.6</v>
+        <v>4.1</v>
       </c>
       <c r="I27" t="n">
-        <v>189244</v>
+        <v>459</v>
       </c>
     </row>
     <row r="28">
@@ -1321,11 +1327,9 @@
           <t>Astound Mobile</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>4.3</v>
-      </c>
+      <c r="C28" t="inlineStr"/>
       <c r="D28" t="n">
-        <v>2955</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
         <v>5</v>
@@ -1334,11 +1338,9 @@
         <v>1</v>
       </c>
       <c r="G28" t="inlineStr"/>
-      <c r="H28" t="n">
-        <v>3.6</v>
-      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
-        <v>2954</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1349,27 +1351,27 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>HT My Account</t>
+          <t>HughesNet Mobile</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="D29" t="n">
-        <v>153532</v>
+        <v>1844</v>
       </c>
       <c r="E29" t="n">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="F29" t="n">
-        <v>20</v>
+        <v>307</v>
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="n">
-        <v>3.6</v>
+        <v>2.8</v>
       </c>
       <c r="I29" t="n">
-        <v>153512</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="30">
@@ -1380,27 +1382,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Google Fiber</t>
+          <t>HT My Account</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3.05</v>
+        <v>2.05</v>
       </c>
       <c r="D30" t="n">
-        <v>1517</v>
+        <v>53</v>
       </c>
       <c r="E30" t="n">
-        <v>3.6</v>
+        <v>1.6</v>
       </c>
       <c r="F30" t="n">
-        <v>291</v>
+        <v>20</v>
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
         <v>2.5</v>
       </c>
       <c r="I30" t="n">
-        <v>1226</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31">
@@ -1411,27 +1413,27 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>My Blue Ridge</t>
+          <t>Midco My Account</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3.55</v>
+        <v>1.85</v>
       </c>
       <c r="D31" t="n">
-        <v>3331</v>
+        <v>287</v>
       </c>
       <c r="E31" t="n">
-        <v>4.6</v>
+        <v>1.3</v>
       </c>
       <c r="F31" t="n">
-        <v>3298</v>
+        <v>24</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="I31" t="n">
-        <v>33</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
@@ -1442,27 +1444,27 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SE Next powered by Tivo</t>
+          <t>Optimum Support</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2.65</v>
+        <v>1.95</v>
       </c>
       <c r="D32" t="n">
-        <v>271</v>
+        <v>2601</v>
       </c>
       <c r="E32" t="n">
-        <v>2.9</v>
+        <v>1.4</v>
       </c>
       <c r="F32" t="n">
-        <v>8</v>
+        <v>1375</v>
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="I32" t="n">
-        <v>263</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="33">
@@ -1473,20 +1475,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Breezeline TV</t>
+          <t>UScellular™ – My Account</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2.65</v>
+        <v>4.25</v>
       </c>
       <c r="D33" t="n">
-        <v>20558</v>
+        <v>48891</v>
       </c>
       <c r="E33" t="n">
-        <v>1.2</v>
+        <v>4.4</v>
       </c>
       <c r="F33" t="n">
-        <v>38</v>
+        <v>28371</v>
       </c>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="n">
@@ -1504,20 +1506,20 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Optimum TV</t>
+          <t>SE Next powered by Tivo</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>3.2</v>
+        <v>2.35</v>
       </c>
       <c r="D34" t="n">
-        <v>13460</v>
+        <v>31</v>
       </c>
       <c r="E34" t="n">
-        <v>4.6</v>
+        <v>2.9</v>
       </c>
       <c r="F34" t="n">
-        <v>13437</v>
+        <v>8</v>
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
@@ -1535,27 +1537,27 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>myBuckeye</t>
+          <t>Optimum TV</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2.8</v>
+        <v>4.1</v>
       </c>
       <c r="D35" t="n">
-        <v>101</v>
+        <v>15893</v>
       </c>
       <c r="E35" t="n">
-        <v>2.5</v>
+        <v>4.6</v>
       </c>
       <c r="F35" t="n">
-        <v>22</v>
+        <v>13437</v>
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="I35" t="n">
-        <v>79</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="36">
@@ -1566,29 +1568,27 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>myCricket App</t>
+          <t>Breezeline TV</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>4.05</v>
+        <v>1.65</v>
       </c>
       <c r="D36" t="n">
-        <v>45606</v>
+        <v>212</v>
       </c>
       <c r="E36" t="n">
-        <v>4.5</v>
+        <v>1.2</v>
       </c>
       <c r="F36" t="n">
-        <v>43149</v>
-      </c>
-      <c r="G36" t="n">
-        <v>90</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
-        <v>3.6</v>
+        <v>2.1</v>
       </c>
       <c r="I36" t="n">
-        <v>2457</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37">
@@ -1599,20 +1599,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>UScellular™ – My Account</t>
+          <t>My Blue Ridge</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4.4</v>
+        <v>4.5</v>
       </c>
       <c r="D37" t="n">
-        <v>29253</v>
+        <v>4180</v>
       </c>
       <c r="E37" t="n">
-        <v>4.4</v>
+        <v>4.6</v>
       </c>
       <c r="F37" t="n">
-        <v>28371</v>
+        <v>3298</v>
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
@@ -1630,27 +1630,27 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Spectrum SportsNet: Live Games</t>
+          <t>myBuckeye</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3.35</v>
+        <v>2.8</v>
       </c>
       <c r="D38" t="n">
-        <v>4323</v>
+        <v>101</v>
       </c>
       <c r="E38" t="n">
-        <v>4.6</v>
+        <v>2.5</v>
       </c>
       <c r="F38" t="n">
-        <v>4149</v>
+        <v>22</v>
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="I38" t="n">
-        <v>174</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>